<commit_message>
adding further variables and descriptions
</commit_message>
<xml_diff>
--- a/Column descriptions.xlsx
+++ b/Column descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milto\Documents\KU Leuven\Data Visualization\data-visualization-course-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708F0522-2129-4626-A96B-C2F987051CAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3168BD2-05AD-4D87-A777-792290598761}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="60" windowWidth="29040" windowHeight="15990" xr2:uid="{42845C4C-90C6-FE4D-9D92-25FCC3B90867}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="128">
   <si>
     <t>Column Name</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>1 Agree 7 Refusal</t>
-  </si>
-  <si>
-    <t>lshshcp</t>
   </si>
   <si>
     <t>little chance to show how capable I am</t>
@@ -800,7 +797,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -816,13 +813,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -833,10 +830,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -847,10 +844,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -864,7 +861,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -878,7 +875,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -892,7 +889,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -906,7 +903,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -920,7 +917,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -934,7 +931,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -953,10 +950,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
@@ -967,10 +964,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>23</v>
@@ -981,212 +978,212 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" t="s">
         <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
       <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
       <c r="C19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
         <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
       <c r="C20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="B21" t="s">
-        <v>51</v>
-      </c>
       <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
       <c r="C22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
         <v>54</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
         <v>57</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
         <v>60</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
         <v>62</v>
-      </c>
-      <c r="B26" t="s">
-        <v>63</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
         <v>64</v>
-      </c>
-      <c r="B27" t="s">
-        <v>65</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1194,13 +1191,13 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
         <v>67</v>
-      </c>
-      <c r="C28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1208,196 +1205,196 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
         <v>69</v>
-      </c>
-      <c r="C29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="C32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="C35" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" t="s">
         <v>110</v>
       </c>
-      <c r="B37" t="s">
-        <v>111</v>
-      </c>
       <c r="C37" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>23</v>
@@ -1405,79 +1402,79 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>